<commit_message>
changed container_type to form_factor
</commit_message>
<xml_diff>
--- a/Projects/INBEVBR_SAND/Data/Ambev template v2.0 - KENGINE.xlsx
+++ b/Projects/INBEVBR_SAND/Data/Ambev template v2.0 - KENGINE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="KPIS" sheetId="1" state="visible" r:id="rId2"/>
@@ -1617,9 +1617,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>5303880</xdr:colOff>
+      <xdr:colOff>5303520</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>75240</xdr:rowOff>
+      <xdr:rowOff>74880</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1632,8 +1632,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="36375840" y="1495440"/>
-          <a:ext cx="4675320" cy="3113640"/>
+          <a:off x="35880480" y="1495440"/>
+          <a:ext cx="4674960" cy="3113280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1659,9 +1659,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>298080</xdr:colOff>
+      <xdr:colOff>297720</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1670,8 +1670,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590400" y="0"/>
-          <a:ext cx="18795600" cy="13176720"/>
+          <a:off x="580680" y="0"/>
+          <a:ext cx="18576360" cy="13176360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1701,9 +1701,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>298080</xdr:colOff>
+      <xdr:colOff>297720</xdr:colOff>
       <xdr:row>81</xdr:row>
-      <xdr:rowOff>60840</xdr:rowOff>
+      <xdr:rowOff>60480</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1712,8 +1712,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590400" y="0"/>
-          <a:ext cx="18795600" cy="13176720"/>
+          <a:off x="580680" y="0"/>
+          <a:ext cx="18576360" cy="13176360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1743,9 +1743,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>923040</xdr:colOff>
+      <xdr:colOff>922680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1754,8 +1754,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590400" y="0"/>
-          <a:ext cx="9600120" cy="161280"/>
+          <a:off x="580680" y="0"/>
+          <a:ext cx="9495360" cy="160920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1785,9 +1785,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>923040</xdr:colOff>
+      <xdr:colOff>922680</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>161280</xdr:rowOff>
+      <xdr:rowOff>160920</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1796,8 +1796,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="590400" y="0"/>
-          <a:ext cx="9600120" cy="161280"/>
+          <a:off x="580680" y="0"/>
+          <a:ext cx="9495360" cy="160920"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1834,14 +1834,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.9744897959184"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.6683673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.469387755102"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="21.0612244897959"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="20.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="73.1632653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.1989795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="20.6530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="19.9795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3329,25 +3330,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.719387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="32.1275510204082"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="50.0816326530612"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="30.1020408163265"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.5714285714286"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="9" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="67.9030612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="29.8316326530612"/>
-    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="58.0459183673469"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="31.7244897959184"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="49.5408163265306"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="29.6989795918367"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="9" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="67.0918367346939"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="29.4285714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="5" customFormat="true" ht="25.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9815,32 +9818,32 @@
   </sheetPr>
   <dimension ref="A1:V114"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="P17" activeCellId="0" sqref="P17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J55" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P85" activeCellId="0" sqref="P85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="95.3061224489796"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="13.5"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="13" min="12" style="5" width="13.5"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="18.8979591836735"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="82.0765306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="24" style="5" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="5" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="5" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="5" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="5" width="94.2244897959184"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="5" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="62.1581632653061"/>
+    <col collapsed="false" hidden="false" max="13" min="12" style="5" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="5" width="18.6275510204082"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="5" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="5" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="19" min="18" style="5" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="5" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="5" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="81.265306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="5" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="24" style="5" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13219,14 +13222,14 @@
       <c r="M78" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O78" s="5" t="s">
-        <v>253</v>
-      </c>
+      <c r="O78" s="0"/>
       <c r="P78" s="0"/>
       <c r="Q78" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="R78" s="0"/>
+      <c r="R78" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="T78" s="5" t="n">
         <v>1</v>
       </c>
@@ -13264,14 +13267,14 @@
       <c r="M79" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O79" s="5" t="s">
-        <v>253</v>
-      </c>
+      <c r="O79" s="0"/>
       <c r="P79" s="0"/>
       <c r="Q79" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="R79" s="0"/>
+      <c r="R79" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="T79" s="5" t="n">
         <v>1</v>
       </c>
@@ -13307,14 +13310,14 @@
       <c r="M80" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O80" s="5" t="s">
-        <v>253</v>
-      </c>
+      <c r="O80" s="0"/>
       <c r="P80" s="0"/>
       <c r="Q80" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="R80" s="0"/>
+      <c r="R80" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="T80" s="5" t="n">
         <v>1</v>
       </c>
@@ -13350,14 +13353,14 @@
       <c r="M81" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O81" s="5" t="s">
-        <v>253</v>
-      </c>
+      <c r="O81" s="0"/>
       <c r="P81" s="0"/>
       <c r="Q81" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="R81" s="0"/>
+      <c r="R81" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="T81" s="5" t="n">
         <v>1</v>
       </c>
@@ -13393,14 +13396,14 @@
       <c r="M82" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O82" s="5" t="s">
-        <v>253</v>
-      </c>
+      <c r="O82" s="0"/>
       <c r="P82" s="0"/>
       <c r="Q82" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="R82" s="0"/>
+      <c r="R82" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="T82" s="5" t="n">
         <v>1</v>
       </c>
@@ -13436,14 +13439,14 @@
       <c r="M83" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="O83" s="5" t="s">
-        <v>253</v>
-      </c>
+      <c r="O83" s="0"/>
       <c r="P83" s="0"/>
       <c r="Q83" s="5" t="n">
         <v>1</v>
       </c>
-      <c r="R83" s="0"/>
+      <c r="R83" s="5" t="s">
+        <v>253</v>
+      </c>
       <c r="T83" s="5" t="n">
         <v>1</v>
       </c>
@@ -14668,39 +14671,38 @@
   </sheetPr>
   <dimension ref="A1:AG104"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="Q24" activeCellId="0" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="37.2602040816326"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="94.8979591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="16.1989795918367"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="25.9183673469388"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="37.6632653061224"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="67.3622448979592"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="16" style="5" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="24" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="82.0765306122449"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="17.280612244898"/>
-    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="41.7142857142857"/>
-    <col collapsed="false" hidden="false" max="29" min="28" style="5" width="20.1122448979592"/>
-    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="13.5"/>
-    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="22.2755102040816"/>
-    <col collapsed="false" hidden="false" max="33" min="33" style="5" width="13.5"/>
-    <col collapsed="false" hidden="false" max="1005" min="34" style="5" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="1006" style="0" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="5" width="36.8520408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="5" width="93.8214285714286"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="5" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="5" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="5" width="25.515306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="5" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="5" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="5" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="5" width="37.2602040816326"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="5" width="66.6836734693878"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="20" min="16" style="5" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="24" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="5" width="81.265306122449"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="5" width="53.8622448979592"/>
+    <col collapsed="false" hidden="false" max="26" min="25" style="5" width="17.0102040816327"/>
+    <col collapsed="false" hidden="false" max="27" min="27" style="5" width="41.1734693877551"/>
+    <col collapsed="false" hidden="false" max="29" min="28" style="5" width="19.8418367346939"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="5" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="5" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="32" min="32" style="5" width="22.0051020408163"/>
+    <col collapsed="false" hidden="false" max="33" min="33" style="5" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1005" min="34" style="5" width="9.98979591836735"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15233,29 +15235,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="49.1377551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="17.1428571428571"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="39.280612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.3826530612245"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="44.9540816326531"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.4387755102041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="29.1581632653061"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="25" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.9285714285714"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="89.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="48.5969387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.8724489795918"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="38.7448979591837"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.1122448979592"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="44.4132653061225"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="19.1683673469388"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="28.7551020408163"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="25" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="0" width="88.6887755102041"/>
+    <col collapsed="false" hidden="false" max="1025" min="26" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18733,7 +18735,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -18759,12 +18761,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="67.6326530612245"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="55.3469387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="66.8214285714286"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="54.6734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>